<commit_message>
first edits done, submitted to christian.
</commit_message>
<xml_diff>
--- a/input/RE.xlsx
+++ b/input/RE.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19200" windowHeight="12180"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cre" sheetId="2" r:id="rId1"/>
     <sheet name="resi" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,6 +107,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF1075A6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -213,7 +218,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="1075A6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -321,11 +326,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="400193392"/>
-        <c:axId val="333266512"/>
+        <c:axId val="379317208"/>
+        <c:axId val="379317600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="400193392"/>
+        <c:axId val="379317208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -362,7 +367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333266512"/>
+        <c:crossAx val="379317600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -370,7 +375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333266512"/>
+        <c:axId val="379317600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400193392"/>
+        <c:crossAx val="379317208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -558,7 +563,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="1075A6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -672,11 +677,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="408996728"/>
-        <c:axId val="408996336"/>
+        <c:axId val="341308720"/>
+        <c:axId val="341307936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="408996728"/>
+        <c:axId val="341308720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,7 +718,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408996336"/>
+        <c:crossAx val="341307936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -721,7 +726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408996336"/>
+        <c:axId val="341307936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +775,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408996728"/>
+        <c:crossAx val="341308720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -909,7 +914,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="1075A6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1023,11 +1028,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="333267688"/>
-        <c:axId val="333268080"/>
+        <c:axId val="372674248"/>
+        <c:axId val="372674640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="333267688"/>
+        <c:axId val="372674248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1069,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333268080"/>
+        <c:crossAx val="372674640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1072,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333268080"/>
+        <c:axId val="372674640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333267688"/>
+        <c:crossAx val="372674248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3061,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:O21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="D6:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3174,8 +3179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>